<commit_message>
adding field gejalaFisik,faktorPendukung,resepObat in excel
</commit_message>
<xml_diff>
--- a/medical_data/dataRumahSakit98.xlsx
+++ b/medical_data/dataRumahSakit98.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7510"/>
+    <workbookView windowWidth="19200" windowHeight="7060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dokter" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>id_dr</t>
   </si>
@@ -55,28 +55,58 @@
     <t>gejala</t>
   </si>
   <si>
+    <t>gejalaFisik</t>
+  </si>
+  <si>
+    <t>faktorPendukung</t>
+  </si>
+  <si>
+    <t>resepObat</t>
+  </si>
+  <si>
     <t>Flu</t>
   </si>
   <si>
     <t>demam,batuk,pilek,sakit kepala</t>
   </si>
   <si>
+    <t>wajah pucat,keringat dingin</t>
+  </si>
+  <si>
+    <t>cuaca dingin</t>
+  </si>
+  <si>
+    <t>paracetamol,antihistamin</t>
+  </si>
+  <si>
+    <t>Diare</t>
+  </si>
+  <si>
+    <t>mual,muntah,sakit perut</t>
+  </si>
+  <si>
+    <t>wajah lesu,dehidrasi</t>
+  </si>
+  <si>
+    <t>makanan tidak higienis</t>
+  </si>
+  <si>
+    <t>oralit,loperamide</t>
+  </si>
+  <si>
     <t>Malaria</t>
   </si>
   <si>
-    <t>demam,menggigil,keringat dingin,sakit kepala,muntah,sakit perut</t>
-  </si>
-  <si>
-    <t>Diare</t>
-  </si>
-  <si>
-    <t>mual,kram perut,perut kembung,lemas,buang air lebih dari 3 kali sehari</t>
-  </si>
-  <si>
-    <t>Demam Berdarah</t>
-  </si>
-  <si>
-    <t>demam tinggi,nyeri otot,mual,muntah,ruam kulit,radang,kelelahan</t>
+    <t>demam,menggigil,keringat dingin</t>
+  </si>
+  <si>
+    <t>dehidrasi,kulit ruam</t>
+  </si>
+  <si>
+    <t>gigitan nyamuk,daerah endemik</t>
+  </si>
+  <si>
+    <t>kina,acetaminophen</t>
   </si>
   <si>
     <t>Gigi Berlubang</t>
@@ -704,9 +734,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1243,7 +1276,7 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1294,53 +1327,92 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="D6 C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="30.8181818181818" customWidth="1"/>
+    <col min="3" max="3" width="24.6363636363636" customWidth="1"/>
+    <col min="4" max="4" width="22.3636363636364" customWidth="1"/>
+    <col min="5" max="5" width="29.4545454545455" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" ht="29" spans="1:5">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1369,18 +1441,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding style, fix history bugs, fix diagnosa phase
</commit_message>
<xml_diff>
--- a/medical_data/dataRumahSakit98.xlsx
+++ b/medical_data/dataRumahSakit98.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7510"/>
+    <workbookView windowWidth="19200" windowHeight="7510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dokter" sheetId="1" r:id="rId1"/>
     <sheet name="GejalaUmum" sheetId="2" r:id="rId2"/>
-    <sheet name="GejalaGigi" sheetId="3" r:id="rId3"/>
+    <sheet name="GejalaGigi" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>id_dr</t>
   </si>
@@ -110,18 +110,6 @@
   </si>
   <si>
     <t>kina,acetaminophen</t>
-  </si>
-  <si>
-    <t>Gigi Berlubang</t>
-  </si>
-  <si>
-    <t>nyeri,sensitivitas,lubang,bengkak</t>
-  </si>
-  <si>
-    <t>Radang Gusi</t>
-  </si>
-  <si>
-    <t>bengkak,bau mulut,akar terlihat,gigi goyah</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1267,7 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1437,39 +1425,14 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="1"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>